<commit_message>
fixes issue #28 adds all codeblocks and imports all required code to run. fixes xls file with an extra row
</commit_message>
<xml_diff>
--- a/code/nst-est2019-0-clean.xlsx
+++ b/code/nst-est2019-0-clean.xlsx
@@ -6,7 +6,7 @@
     <sheet state="visible" name="NST01" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_NST01">'NST01'!$A$2:$L$53</definedName>
+    <definedName name="_NST01">'NST01'!$A$2:$L$52</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
@@ -2943,42 +2943,18 @@
       <c r="Y52" s="3"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="4">
-        <v>3725789.0</v>
-      </c>
-      <c r="B53" s="4">
-        <v>3726157.0</v>
-      </c>
-      <c r="C53" s="4">
-        <v>3721525.0</v>
-      </c>
-      <c r="D53" s="4">
-        <v>3678732.0</v>
-      </c>
-      <c r="E53" s="4">
-        <v>3634488.0</v>
-      </c>
-      <c r="F53" s="4">
-        <v>3593077.0</v>
-      </c>
-      <c r="G53" s="4">
-        <v>3534874.0</v>
-      </c>
-      <c r="H53" s="4">
-        <v>3473232.0</v>
-      </c>
-      <c r="I53" s="4">
-        <v>3406672.0</v>
-      </c>
-      <c r="J53" s="4">
-        <v>3325286.0</v>
-      </c>
-      <c r="K53" s="4">
-        <v>3193354.0</v>
-      </c>
-      <c r="L53" s="4">
-        <v>3193694.0</v>
-      </c>
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
@@ -8366,33 +8342,7 @@
       <c r="X252" s="3"/>
       <c r="Y252" s="3"/>
     </row>
-    <row r="253" ht="15.75" customHeight="1">
-      <c r="A253" s="3"/>
-      <c r="B253" s="3"/>
-      <c r="C253" s="3"/>
-      <c r="D253" s="3"/>
-      <c r="E253" s="3"/>
-      <c r="F253" s="3"/>
-      <c r="G253" s="3"/>
-      <c r="H253" s="3"/>
-      <c r="I253" s="3"/>
-      <c r="J253" s="3"/>
-      <c r="K253" s="3"/>
-      <c r="L253" s="3"/>
-      <c r="M253" s="3"/>
-      <c r="N253" s="3"/>
-      <c r="O253" s="3"/>
-      <c r="P253" s="3"/>
-      <c r="Q253" s="3"/>
-      <c r="R253" s="3"/>
-      <c r="S253" s="3"/>
-      <c r="T253" s="3"/>
-      <c r="U253" s="3"/>
-      <c r="V253" s="3"/>
-      <c r="W253" s="3"/>
-      <c r="X253" s="3"/>
-      <c r="Y253" s="3"/>
-    </row>
+    <row r="253" ht="15.75" customHeight="1"/>
     <row r="254" ht="15.75" customHeight="1"/>
     <row r="255" ht="15.75" customHeight="1"/>
     <row r="256" ht="15.75" customHeight="1"/>
@@ -9138,7 +9088,6 @@
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>

</xml_diff>